<commit_message>
añadir nombre a las restricciones y terminar el diccionario completo de lectura de datos
</commit_message>
<xml_diff>
--- a/data/datos2.xlsx
+++ b/data/datos2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Desktop\flexible-vrp-feature-base_mip\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFG\flexible-vrp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EEEC7F7-C89D-4358-BD7D-9456312CC5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA17DB92-DDD4-452B-B697-4F2A012C4F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -101,12 +101,15 @@
   </si>
   <si>
     <t>required</t>
+  </si>
+  <si>
+    <t>warehouse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,19 +522,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -547,7 +550,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -555,7 +558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -563,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -571,7 +574,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -579,7 +582,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -587,7 +590,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -595,7 +598,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -603,7 +606,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -618,52 +621,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -674,16 +682,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -694,7 +702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -705,7 +713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -716,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -727,7 +735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -738,7 +746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -749,7 +757,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -760,7 +768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -771,7 +779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -782,7 +790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -793,7 +801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -804,7 +812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -815,7 +823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -826,7 +834,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -837,7 +845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -848,7 +856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -859,7 +867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -870,7 +878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -881,7 +889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -892,7 +900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -903,7 +911,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -914,7 +922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -925,7 +933,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -936,7 +944,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -947,7 +955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -958,7 +966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -969,7 +977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -980,7 +988,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -991,7 +999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1002,7 +1010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1013,7 +1021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -1024,7 +1032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1035,7 +1043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -1046,7 +1054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1057,7 +1065,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -1068,7 +1076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1079,7 +1087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1090,7 +1098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1101,7 +1109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1112,7 +1120,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1123,7 +1131,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1134,7 +1142,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -1145,7 +1153,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1156,7 +1164,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1167,7 +1175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1178,7 +1186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1189,7 +1197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1200,7 +1208,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1211,7 +1219,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1222,7 +1230,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1233,7 +1241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -1244,7 +1252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -1255,7 +1263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -1266,7 +1274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -1277,7 +1285,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -1288,7 +1296,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -1299,7 +1307,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -1317,14 +1325,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1338,7 +1348,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1352,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1363,10 +1373,10 @@
         <v>37</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1380,7 +1390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1394,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1405,10 +1415,10 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1419,10 +1429,10 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1436,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1450,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1461,10 +1471,10 @@
         <v>28</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1475,10 +1485,10 @@
         <v>11</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1490,6 +1500,160 @@
       </c>
       <c r="D12">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>102</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>105</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>58</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>91</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>34</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eliminamos la hoja de warehouses
</commit_message>
<xml_diff>
--- a/data/datos2.xlsx
+++ b/data/datos2.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFG\flexible-vrp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA17DB92-DDD4-452B-B697-4F2A012C4F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D71EB8-49F7-4CDF-8F82-1C69EB328312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
-    <sheet name="warehouse" sheetId="2" r:id="rId2"/>
-    <sheet name="trip_duration" sheetId="3" r:id="rId3"/>
-    <sheet name="comp_quantity_inst1" sheetId="4" r:id="rId4"/>
+    <sheet name="trip_duration" sheetId="3" r:id="rId2"/>
+    <sheet name="comp_quantity_inst1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -101,9 +100,6 @@
   </si>
   <si>
     <t>required</t>
-  </si>
-  <si>
-    <t>warehouse</t>
   </si>
 </sst>
 </file>
@@ -621,67 +617,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C57"/>
   <sheetViews>
@@ -1324,7 +1259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>

</xml_diff>